<commit_message>
Added Comments and madefinal changes
</commit_message>
<xml_diff>
--- a/agency_websites.xlsx
+++ b/agency_websites.xlsx
@@ -443,315 +443,315 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.whiteriversmedia.com/</t>
+          <t>https://echovme.in/</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.mandywebdesign.com/</t>
+          <t>https://socialpanga.com/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.brandloom.com/</t>
+          <t>https://www.matebiz.com/</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.digidarts.com/</t>
+          <t>https://clutch.co/in/web-designers</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.ezrankings.com/seo-company-india.html</t>
+          <t>https://www.matebiz.com/digital-marketing-service/</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.designrush.com/agency/search-engine-optimization/in</t>
+          <t>https://webeesocial.com/</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.rankingbyseo.com/</t>
+          <t>https://seoexpertscompanyindia.com/</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://www.vocso.com/</t>
+          <t>https://www.designrush.com/agency/website-design-development/in</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://www.aoneseoservice.com/</t>
+          <t>https://www.designrush.com/agency/search-engine-optimization/in</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://www.webhopers.com/top-web-designing-companies-in-india</t>
+          <t>https://www.mandywebdesign.com/</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://echovme.in/</t>
+          <t>https://www.seotonic.com/</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://www.seotonic.com/</t>
+          <t>https://www.ezrankings.com/seo-company-india.html</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://indiawebdesigns.in/</t>
+          <t>https://www.designrush.com/agency/digital-agencies/in</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://socialpanga.com/</t>
+          <t>https://www.socialee.in/</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://omrdigital.com/</t>
+          <t>https://www.foduu.com/</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://webeesocial.com/</t>
+          <t>https://www.webhopers.com/top-web-designing-companies-in-india</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://www.foduu.com/</t>
+          <t>https://www.digitalsilk.com/</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>https://www.ezrankings.com/web-design-company-india.html</t>
+          <t>https://www.webhopers.com/seo-company-india</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>https://www.aalpha.net/services/design-services/web-design-india/</t>
+          <t>https://acodez.in/</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>https://seoexpertscompanyindia.com/</t>
+          <t>https://omrdigital.com/</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>https://www.semrush.com/agencies/list/seo/india/</t>
+          <t>https://www.digidarts.com/</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>https://seoserviceinindia.co.in/</t>
+          <t>https://www.whiteriversmedia.com/</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/pulse/top-10-digital-marketing-agencies-india-socialee-wldmf</t>
+          <t>https://www.vocso.com/</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>https://www.techmagnate.com/</t>
+          <t>https://www.brandloom.com/</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>https://noviindus.com/web-designing-company-india/</t>
+          <t>https://www.seodiscovery.com/seo-company-india.php</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>https://www.designrush.com/agency/digital-agencies/in</t>
+          <t>https://www.mumbaiwebdesign.in/</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>https://www.mumbaiwebdesign.in/</t>
+          <t>https://colorwhistle.com/</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>https://colorwhistle.com/</t>
+          <t>https://www.ezrankings.com/web-design-company-india.html</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>https://www.webhopers.com/seo-company-india</t>
+          <t>https://florafountain.com/</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>https://www.matebiz.com/digital-marketing-service/</t>
+          <t>https://www.linkedin.com/pulse/top-10-digital-marketing-agencies-india-socialee-wldmf</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>https://www.seodiscovery.com/seo-company-india.php</t>
+          <t>https://www.pixelcrayons.com/services/digital-marketing/seo</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>https://wefttechnologies.com/digital-marketing-company-in-india/</t>
+          <t>https://thatware.co/seo-company-india/</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>https://the7eagles.com/india/seo-company/</t>
+          <t>https://www.aoneseoservice.com/</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>https://clutch.co/in/web-designers</t>
+          <t>https://indiawebdesigns.in/</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>https://thatware.co/seo-company-india/</t>
+          <t>https://www.aaravinfotech.com/web-design-services.php</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>https://www.socialee.in/</t>
+          <t>https://www.rankontechnologies.com/seo-services/</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>https://www.orangemantra.com/services/search-engine-optimization/</t>
+          <t>https://www.techmagnate.com/</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>https://www.matebiz.com/</t>
+          <t>https://seoserviceinindia.co.in/</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>https://www.designrush.com/agency/website-design-development/in</t>
+          <t>https://www.semrush.com/agencies/list/seo/india/</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>https://www.neelnetworks.com/</t>
+          <t>https://www.ezrankings.com/</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>https://pwskills.com/blog/digital-marketing-companies/</t>
+          <t>https://www.rankingbyseo.com/</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>https://www.ezrankings.com/</t>
+          <t>https://pwskills.com/blog/digital-marketing-companies/</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>https://www.rankontechnologies.com/seo-services/</t>
+          <t>https://noviindus.com/web-designing-company-india/</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>https://acodez.in/</t>
+          <t>https://www.orangemantra.com/services/search-engine-optimization/</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>https://florafountain.com/</t>
+          <t>https://wefttechnologies.com/digital-marketing-company-in-india/</t>
         </is>
       </c>
     </row>

</xml_diff>